<commit_message>
For each class label
</commit_message>
<xml_diff>
--- a/statistic/document.xlsx
+++ b/statistic/document.xlsx
@@ -219,6 +219,9 @@
     <t>Başbakan Yıldırım: Bu ihanet çetesini milletimizin gücü etkisiz hale getirecektir. Çok aptalca, çılgınca bir girişimdir.</t>
   </si>
   <si>
+    <t>27 Şubat, Gregoryen Takvimi'ne göre yılın 58. günüdür. Yıl sonuna kadar kalan 307 gün vardır (artık yıllarda 308).</t>
+  </si>
+  <si>
     <t>😍😍Açık Büfe #Kahvaltı - Bambi Garden/ #İstanbul ( #Üsküdar )
 🍳 Kahvaltı Servis Saati 10:00 - 14:00
 💵 35₺/ Kişi Başı
@@ -434,9 +437,6 @@
   </si>
   <si>
     <t>27/02/1964 - Coca-Cola'nın dünya üzerindeki 1916'ncı fabrikası İstanbul'da açıldı. https://t.co/XZUasvKkp4</t>
-  </si>
-  <si>
-    <t>27 Şubat, Gregoryen Takvimi'ne göre yılın 58. günüdür. Yıl sonuna kadar kalan 307 gün vardır (artık yıllarda 308).</t>
   </si>
   <si>
     <t>26/02/1992 - Hocalı Katliamı; Azerbaycan'ın Hocalı kentine giren silahlı Ermeni gruplar 613 Azeri'yi öldürdü. https://t.co/nyHvBuOJxm</t>
@@ -853,7 +853,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B139"/>
+  <dimension ref="A1:B140"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1839,7 +1839,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>122</v>
+        <v>53</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -1847,7 +1847,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -1855,7 +1855,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -1863,7 +1863,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -1871,7 +1871,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -1879,7 +1879,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -1887,7 +1887,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -1895,7 +1895,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -1903,7 +1903,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -1911,7 +1911,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -1919,7 +1919,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -1927,7 +1927,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -1935,7 +1935,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -1943,7 +1943,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -1951,7 +1951,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -1959,7 +1959,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -1967,6 +1967,14 @@
         <v>137</v>
       </c>
       <c r="B139" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="B140" t="s">
         <v>138</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update,fix,news tokenizer added,dbupdated with news tokenizer
</commit_message>
<xml_diff>
--- a/statistic/document.xlsx
+++ b/statistic/document.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="257">
   <si>
     <t>tweet</t>
   </si>
@@ -108,6 +108,9 @@
     <t>25/02/1836 - Samuel Colt, ürettiği silahın (Colt (tabanca)) patentini aldı.</t>
   </si>
   <si>
+    <t>18/12/1865 - ABD'de kölelik kaldırıldı.</t>
+  </si>
+  <si>
     <t>30/10/1973 - Boğaziçi Köprüsü, Cumhurbaşkanı Fahri Korutürk tarafından açıldı.</t>
   </si>
   <si>
@@ -120,9 +123,36 @@
     <t>30/09/1964 - Oyuncu ve eski model Monica Belluci İtalya'da doğdu. https://t.co/WV0LmPZJ93</t>
   </si>
   <si>
+    <t>16/09/1953 - İlk sinemaskop film gösterimi New York'ta yapıldı.</t>
+  </si>
+  <si>
+    <t>14/09/1944 - Radyo istasyonlarının kurulması ve genişletilmesi yasası çıktı.</t>
+  </si>
+  <si>
     <t>30/08/1952 - Erzurum'da Aziziye Anıtı açıldı.</t>
   </si>
   <si>
+    <t>27/08/1859 - Dünyanın ilk petrol kuyusu ABD’nin Pensilvanya eyaletinde açıldı.</t>
+  </si>
+  <si>
+    <t>09/08/1928 - Arap Alfabesi yerine Latin Alfabesi'nin benimsendiği Harf Devrimi gerçekleştirildi.</t>
+  </si>
+  <si>
+    <t>11/05/1924 - Gottlieb Daimler ve Karl Benz şiketleri birleşerek Mercedes-Benz şirketini oluşturdular.</t>
+  </si>
+  <si>
+    <t>10/04/1912 - RMS Titanic ilk seferine çıktı. https://t.co/EiqZkZRDD6</t>
+  </si>
+  <si>
+    <t>20/02/1872 - Metropolitan Museum of Art, New York'ta açıldı. https://t.co/jKW7n0oenO</t>
+  </si>
+  <si>
+    <t>14/02/1982 - Oyuncu Özge Borak İstanbul'da doğdu. https://t.co/6wOKVQXlLW</t>
+  </si>
+  <si>
+    <t>İzmir'de de okullar tatil edildi.</t>
+  </si>
+  <si>
     <t>23/12/1954 - İlk organ nakli (böbrek) Boston'da gerçekleştirildi.</t>
   </si>
   <si>
@@ -138,16 +168,54 @@
     <t>#DünyaBarışGünü https://t.co/vWahJTBMFx</t>
   </si>
   <si>
+    <t>07/09/1782 - William Herschel kendi tasarımı olan teleskopla Satürn Bulutsusunu keşfetti. https://t.co/3slWmqotOx</t>
+  </si>
+  <si>
+    <t>24/07/1923 - Lozan Antlaşması imzalandı.</t>
+  </si>
+  <si>
     <t>#AliİsmailKorkmaz https://t.co/73E5e8ZWGe</t>
   </si>
   <si>
     <t>08/07/1621 - Yazar La Fontaine Fransa'da doğdu. (ö. 1695) https://t.co/3KqukXuIpX</t>
   </si>
   <si>
+    <t>05/05/1474 - Kristof Kolomb Jamaika Adasına ayak bastı ve adaya Santa Gloria adını verdi.</t>
+  </si>
+  <si>
+    <t>15/04/1929 - İstanbul'da terzilik mektebi açıldı.</t>
+  </si>
+  <si>
     <t>27/03/1994 - Eurofighter Typhoon ilk test uçuşunu yaptı. https://t.co/sNKlbJpfo5</t>
   </si>
   <si>
+    <t>06/03/1869 - Dimitri Mendeleyev, ilk periyodik tabloyu açıkladı. https://t.co/BkXdNnepj9</t>
+  </si>
+  <si>
+    <t>09/02/1621 - İstanbul Boğazı dondu. https://t.co/fkR5vpo5fq</t>
+  </si>
+  <si>
     <t>04/02/1902 - Paris'te Birinci Jön Türk Kongresi yapıldı. https://t.co/PFKnnkRn4T</t>
+  </si>
+  <si>
+    <t>Isslama #Köfte - Isslama Köfte / İstanbul ( #Acıbadem, #Ataşehir ) 
+🕦 Çalışma Saatleri 11:00 - 22:00
+☎ 444 10 06
+💵 19,50₺/ 1 Porsiyon
+💵 27,50₺/ 1,5 Porsiyon
+📹 1,5 Porsiyon
+🍹Alkolsüz Mekan
+🚲 Paket Servis Var
+#yemekneredeyenircom https://t.co/ucXhAu6eVz</t>
+  </si>
+  <si>
+    <t>Dördü Bir Arada Atom - #Künefe Cenneti / İstanbul (#Mahmutbey - #Kocasinan) 
+🕦 Çalışma Saatleri 10:00-02:00
+☎ 0 212 630 97 44 
+💵 70₺ / 4 Kişilik 
+💵 102₺ / 6 Kişilik
+📹 4 Kişilik 
+#yemekneredeyenircom https://t.co/yvD9EEDYRf</t>
   </si>
   <si>
     <t>#Kebap Çeşitleri - Akcanlar Ocakbaşı / #İstanbul (#Elmadağ -#Şişli)
@@ -162,6 +230,26 @@
 #yemekneredeyenircom https://t.co/eRtN0JNcZm</t>
   </si>
   <si>
+    <t>#Ciğer Şiş  - Hanek Gaziantep Sofrası / #İstanbul ( #Koşuyolu ) 
+🕦 Çalışma Saatleri 09:30 - 22:00
+☎ 0216 340 23 40
+💵 32₺
+🍹 Alkolsüz Mekan 
+🚴 Paket Servis Var
+💳 Sodexo, Ticket, Multinet, Setcard Var
+#yemekneredeyenircom https://t.co/SfbXmGBzpJ</t>
+  </si>
+  <si>
+    <t>Cevizzade - Künefe Cenneti / #İstanbul (#Mahmutbey - #Kocasinan)
+🕦 Çalışma Saatleri 10:00-02:00
+☎ 0 212 630 97 44 
+💵 17₺ / 1 Kişilik 
+💵 65₺ / 4 Kişilik 
+💵 95₺ / 6 Kişilik 
+📹 4 Kişilik 
+#yemekneredeyenircom https://t.co/lxZZOIguCk</t>
+  </si>
+  <si>
     <t>#Çorba Çeşitleri - Baruthane Pilavcısı/#İstanbul (#Kurtuluş)
 ☎ 0 212 296 01 02
 💵 7₺ / Ezogelin Çorbası
@@ -204,6 +292,26 @@
 #yemekneredeyenircom https://t.co/LKNowO8gE8</t>
   </si>
   <si>
+    <t>RT @basakmaviss: Dost gerçekten de kara günde belli oluyor ❤️ https://t.co/ucBG5iCnz1</t>
+  </si>
+  <si>
+    <t>Ağlayan Pasta &amp;amp; Kaymaklı Ayva Tatlısı - Prasini Papia Cafe / İstanbul ( Gayrettepe ) 
+🕦 Çalışma Saatleri Hafta İçi 06:30 - 19:00
+🕦 Çalışma Saatleri Cumartesi 09:00 - 17:00
+☎ 0 533 138 65 46
+💵 14₺/ Kaymaklı Ayva Tatlısı
+💵 14₺/ Ağlayan Pasta
+#yemekneredeyenircom https://t.co/62KIdxDFRq</t>
+  </si>
+  <si>
+    <t>Havuç Dilim - Cihan Et Kasap Pişiricisi  /  (#İzmir - Forum Bornova Karşısı) 
+🕦 Çalışma Saatleri 11:00-23:00
+☎ 0 232 469 19 56 
+💵 14₺ Porsiyon 
+💵 17₺ /  Dondurmalı 
+#yemekneredeyenircom https://t.co/eLg1vOKupb</t>
+  </si>
+  <si>
     <t>@pelinkrkc Gel, günaha girelim 😎</t>
   </si>
   <si>
@@ -216,10 +324,35 @@
     <t>RT @dilarataogllu: Yemekneredeyenircom'a uzun uzun bakıp ic gecirdiğimiz saatlere hosgeldiniz</t>
   </si>
   <si>
+    <t>Yumurta Çeşitleri - Coşkun Et / İstanbul ( İstoç, Kağıthane, Bağcılar )
+💵 18₺/ Kahvaltı Tabağı
+💵 13₺/ Yumurtalı #Kavurma
+#yemekneredeyenir https://t.co/uhWRh8ddNI</t>
+  </si>
+  <si>
+    <t>Nam nam 😇
+İsli Dana Bacon Burger - #Hamburger Kafası / #İstanbul ( #Cihangir #Firuzağa İlkokulu Yanı )
+💵 40₺/ 220 Gram
+#yemekneredeyenir https://t.co/RK3Y6xCIuZ</t>
+  </si>
+  <si>
+    <t>Her yerimiz hamburger 😅
+Mantar Burger - Hamburger Kafası / İstanbul ( #Cihangir #Firuzağa İlkokulu Yanı ) 
+💵 20₺/ 110 Gram
+#yemekneredeyenir https://t.co/YU1HaU96hg</t>
+  </si>
+  <si>
     <t>Başbakan Yıldırım: Bu ihanet çetesini milletimizin gücü etkisiz hale getirecektir. Çok aptalca, çılgınca bir girişimdir.</t>
   </si>
   <si>
     <t>27 Şubat, Gregoryen Takvimi'ne göre yılın 58. günüdür. Yıl sonuna kadar kalan 307 gün vardır (artık yıllarda 308).</t>
+  </si>
+  <si>
+    <t>Günaydın 😍
+Serpme Köy Kahvaltısı - Ayder Sofrası #İstanbul ( #Sarıyer )
+💵 25₺ / Kavurma
+💵 40₺/ Kişi Başı
+#yemekneredeyenir https://t.co/DIDFAkmzYo</t>
   </si>
   <si>
     <t>😍😍Açık Büfe #Kahvaltı - Bambi Garden/ #İstanbul ( #Üsküdar )
@@ -234,6 +367,18 @@
 #yemekneredeyenir https://t.co/XR8HpU2ymM</t>
   </si>
   <si>
+    <t>@yarentheminnok Ölümlü dünya aman boşver 😛</t>
+  </si>
+  <si>
+    <t>Rengarenk 🎈 Ara Sıcaklar &amp;amp; Meze Çeşitleri - Balıkçı Hüseyin Usta / İzmir ( Forum Bornova Girişi )
+Detaylı Bilgi: https://t.co/X2DnKpVc1S https://t.co/Vd9vOYB4Y1</t>
+  </si>
+  <si>
+    <t>Yaklaşık 1 saattir bakışıyoruz 🤗 #SerpmeKahvaltı Seven Hills Restaurant #İstanbul #Sultanahmet
+☎️ 0 212 516 94 97
+💵 50₺/ Kişi Başı https://t.co/vJso77fzb6</t>
+  </si>
+  <si>
     <t>#Günaydın ☺️ Bam's Sıcak Kahvaltı &amp;amp; Bam's Klasik #Kahvaltı Bam's Cafe Restaurant #İstanbul #Acıbadem https://t.co/kkn8PdNRyu</t>
   </si>
   <si>
@@ -242,6 +387,12 @@
 💵 10₺ https://t.co/11EBuwvrBr</t>
   </si>
   <si>
+    <t>Acıktık 🤓 #EtliWrap Coffee Shop Company #Adana ( Uğrum Mumcu Bulvarı, M1 AVM )
+🕦 Çalışma Saatleri 08:30-00:00
+☎ 0 322 235 33 01
+💵 24,50₺ https://t.co/JXalys3Klt</t>
+  </si>
+  <si>
     <t>Severiz ❤️
 Samsalı Serpme Kahvaltı - Dumanti / İstanbul #Halkalı #kahvaltı▫ https://t.co/v2lVd5s0Db</t>
   </si>
@@ -256,12 +407,22 @@
 💵 44₺ / 200 Gram https://t.co/Tvv6wuG23v</t>
   </si>
   <si>
+    <t>Eridik 😐 Beyran - Kimyon / İstanbul #Moda #KadifeSokak #beyran https://t.co/jx50JySyxb</t>
+  </si>
+  <si>
     <t>Vakti gelmişti 👊🏻 Et Döner - Parça Döner / İstanbul (Beşiktaş) https://t.co/ElURgTnbfS</t>
   </si>
   <si>
+    <t>Etçiler burada mı ? 
+Shatobiryan - Shato Steakhouse #İstanbul Yıldırım #Bayrampaşa https://t.co/4qESO0xB5f</t>
+  </si>
+  <si>
     <t>TCMB: KAPASİTE KULLANIM ORANI MART'TA YÜZDE 77,8 (ÖNCEKİ YÜZDE 77,8)</t>
   </si>
   <si>
+    <t>BORSA İSTANBUL GÜNÜ YÜZDE 1.51 ORANINDA DÜŞÜŞLE 115 BİN 450 PUANDAN TAMAMLADI</t>
+  </si>
+  <si>
     <t>Polis koleji sınavında usulsüzlük operasyonu - https://t.co/rsYTMkyAjX https://t.co/5nPnlkH7aF</t>
   </si>
   <si>
@@ -271,27 +432,78 @@
     <t>İsrail'de askerlik krizi - https://t.co/LAwMWjsmS7 https://t.co/hmGiNLRL5T</t>
   </si>
   <si>
+    <t>Putin'e muhalif isim İngiltere'de ölü bulundu - https://t.co/4mTHepzSU1 https://t.co/VXM3Dkdoho</t>
+  </si>
+  <si>
     <t>Fenerbahçe'den Alex açıklaması - https://t.co/EE2lyeyq6I https://t.co/cd5GUqVAuu</t>
   </si>
   <si>
+    <t>ABD: Türkiye ile Afrin sorununu çözmeye çalışıyoruz - https://t.co/eaepiPMxB3 https://t.co/JUB7QYnCbs</t>
+  </si>
+  <si>
     <t>Yolcu bıçaklayan taksiciye 1.5 yıl hapis cezası istendi - https://t.co/fnpToJLYKP https://t.co/jWRfPvP4mo</t>
   </si>
   <si>
+    <t>Fenerbahçe, Zalgiris Kaunas'ı mağlup etti - https://t.co/75ZJIqG9Cg https://t.co/aeDUz1bJup</t>
+  </si>
+  <si>
     <t>ABD'de silahlı saldırı! Rehineler var - https://t.co/gELVoSvXcR https://t.co/Am8Y1Za7yu</t>
   </si>
   <si>
     <t>Morgan Stanley: Dolar zayıflayacak - https://t.co/QxJLGBlRDz https://t.co/BLQ7yTH8gI</t>
   </si>
   <si>
+    <t>Emekliye 224 TL zam - https://t.co/djTIAcfnIP https://t.co/DnHihZhebD</t>
+  </si>
+  <si>
+    <t>TSK, Cinderes merkezini ele geçirdi - https://t.co/fpdpTuJiwn https://t.co/PipDFuxQg4</t>
+  </si>
+  <si>
+    <t>Raci Şaşmaz Denge'de alım yapıyor - https://t.co/IgB6bSZ0JS https://t.co/O2PfcoAe5z</t>
+  </si>
+  <si>
+    <t>ÖİB o ihale için yeniden süre uzattı - https://t.co/RzaqzMndF3 https://t.co/MNzpZtvUNs</t>
+  </si>
+  <si>
+    <t>Dallas Fed Başkanı'ndan NAFTA uyarısı - https://t.co/cprQUjeOH6 https://t.co/DtfewSRYum</t>
+  </si>
+  <si>
+    <t>Türk dizilerinin yayından kaldırılışında Prens parmağı mı var - https://t.co/ls0bwgMxmr https://t.co/HG7MECFyTQ</t>
+  </si>
+  <si>
     <t>Teşvik döneminde 1 milyonu aşkın istihdam gerçekleşti - https://t.co/UGomlYV5zQ https://t.co/kafWEoIZE1</t>
   </si>
   <si>
+    <t>Sivas'taki FETÖ'cüler tutuklandı - https://t.co/6v2m5kyMgx https://t.co/8biiaoypbh</t>
+  </si>
+  <si>
+    <t>Trump'a Amerikan iş dünyasından ek gümrük vergisi tepkisi - https://t.co/4fTdElQenU https://t.co/wsAvq1DEim</t>
+  </si>
+  <si>
+    <t>Erdoğan: 2348 terörist etkisiz hale getirildi - https://t.co/ujGq4Buh9e https://t.co/10pm6b6KF1</t>
+  </si>
+  <si>
+    <t>BORSA İSTANBUL GÜNÜ YÜZDE 0.66 ORANINDA DÜŞÜŞLE 116 BİN 859 PUANDAN KAPADI</t>
+  </si>
+  <si>
+    <t>Salih Müslim'e her durakta kırmızı bülten - https://t.co/cwmpGWhm3D https://t.co/mK3AZpd5gQ</t>
+  </si>
+  <si>
+    <t>Bosna Hersek'e EBRD'den 750 milyon euro kredi - https://t.co/rMd8Mxxo0w https://t.co/fSheKOSavS</t>
+  </si>
+  <si>
+    <t>Akdağ çocuk istismarında öngörülen cezayı açıkladı - https://t.co/1HYK0GQO7N https://t.co/H3dIfU8yB7</t>
+  </si>
+  <si>
     <t>KRGYO: Karlılığı azaldı - https://t.co/zAetWnXMOW https://t.co/47K89xQFS4</t>
   </si>
   <si>
     <t>Arap basınından müthiş takas iddiası - https://t.co/2XUZx5E0jt https://t.co/6K2AlMz8z1</t>
   </si>
   <si>
+    <t>Tahliye edildi ABD’ye kaçtı - https://t.co/cJ8eGqx4Ti https://t.co/F9UTrW1O36</t>
+  </si>
+  <si>
     <t>Borsa İstanbul yükselişle açıldı - https://t.co/XkzeYUetO1 https://t.co/NMMxj6XGs0</t>
   </si>
   <si>
@@ -301,6 +513,9 @@
     <t>CHP'den istifa edip AK Parti'ye geçtiler - https://t.co/T85AzpRNZI https://t.co/ANO3EhVKYG</t>
   </si>
   <si>
+    <t>Metro Holding'in 2017 karı bir önceki yıla göre %397 arttı - https://t.co/sloMSddi8M https://t.co/i9oG50NKf5</t>
+  </si>
+  <si>
     <t>Milyonları ilgilendiren düzenleme haftaya Meclis'te - https://t.co/wfc4e35wiD https://t.co/cLjbscebGL</t>
   </si>
   <si>
@@ -310,36 +525,114 @@
     <t>Ali Koç Aziz Yıldırım'a meydan okudu - https://t.co/GFlbLLfhJS https://t.co/EaxfXI8NKZ</t>
   </si>
   <si>
+    <t>ABD borsaları düştü, küresel piyasalar karışık seyretti - https://t.co/cznncCvKBl https://t.co/zJDEppGmmn</t>
+  </si>
+  <si>
+    <t>Rekor! 2017'de 1 milyon 323 bin konuta ruhsat  - https://t.co/zJeu3o269C https://t.co/Hq1N4vfo1L</t>
+  </si>
+  <si>
+    <t>İttifakın ince ayrıntıları - https://t.co/D2hjUILa5E https://t.co/ydE58t4YOC</t>
+  </si>
+  <si>
+    <t>Erdoğan ile Putin görüştü - https://t.co/jUUV0C0kb8 https://t.co/XpfueD5zUa</t>
+  </si>
+  <si>
+    <t>Türkiye'de ilk kez! Yerli şanzıman - https://t.co/o3rTn3E8gp https://t.co/EkP8kPJYy9</t>
+  </si>
+  <si>
+    <t>Balkaya Pastanesi ( Balıkesir ) #bugunnereyegitsem https://t.co/6HwE9WtbAc</t>
+  </si>
+  <si>
     <t>Maharet Döner ( İzmir , Bayraklı ) #bugunnereyegitsem @maharetdoner @ Maharet Döner https://t.co/YdSBHqsVTY</t>
   </si>
   <si>
+    <t>Manufaktura , Belgrade #bugunnereyegitsem @ Manufaktura Belgrade https://t.co/b4zEBgByS0</t>
+  </si>
+  <si>
     <t>Daha iyisi yok 💪🏼👊🏼 Öz İkizler Künefe ( Gaziantep ) #bugunnereyegitsem @ Öz İkizler Künefe https://t.co/2BgJqE5IeS</t>
   </si>
   <si>
     <t>İmam Çağdaş ( Gaziantep ) #bugunnereyegitsem @ İmam Çağdaş https://t.co/19F61Vb0Y9</t>
   </si>
   <si>
+    <t>Gönül Kahvesi ( Caddebostan ) #bugunnereyegitsem @ Gönül Kahvesi-Caddebostan https://t.co/FmPgYytp9u</t>
+  </si>
+  <si>
+    <t>Kemal Usta Waffle ( Erenköy ) #bugunnereyegitsem @ Kemal Usta Waffles Erenköy https://t.co/gIQr87ge20</t>
+  </si>
+  <si>
+    <t>The Galliard ( Etiler ) #bugunnereyegitsem @ersinsuzer thegalliard #14subat @ The GALLIARD https://t.co/6p2fD8WDds</t>
+  </si>
+  <si>
+    <t>Nar Bahçesi ( Çengelköy ) #bugunnereyegitsem @narbahcesicafe @ Nar Bahçesi https://t.co/r1orYJZxnY</t>
+  </si>
+  <si>
+    <t>#iyigeceler #arkadaslarinizietiketleyin 😍😁 https://t.co/y7QWZBGEPL</t>
+  </si>
+  <si>
+    <t>3 Adamı İzleyenler el kaldırsın ✋🏼😁 @ Sur Yapı Exen İstanbul https://t.co/Yp1U9qsQti</t>
+  </si>
+  <si>
+    <t>Lacivert Restaurant ( Anadoluhisarı ) #bugunnereyegitsem @ Lacivert https://t.co/ZyMyt7zH1m</t>
+  </si>
+  <si>
+    <t>Sevdiklerinizi Mutlu Edin 😍 ciceksepeti #ciceksepeti #bng https://t.co/yiuql5aTYx</t>
+  </si>
+  <si>
+    <t>Cumartesi klasiği Dürümcü Emmi'de Beyran 🙊 @ Dürümcü Emmi https://t.co/euovdrRcg4</t>
+  </si>
+  <si>
+    <t>Sapphire Istanbul ( 4.Levent ) #bugunnereyegitsem #bng @ Sapphire İstanbul https://t.co/GvimGwsgPJ</t>
+  </si>
+  <si>
+    <t>Sapphire Istanbul #bugunnereyegitsem @ İstanbul Sapphire Seyir Terasi https://t.co/TOM98qVGt0</t>
+  </si>
+  <si>
+    <t>34,5 Ege Fast Food ( Koşuyolu ) #bugunnereyegitsem #bng @ 34,5 Ege Fast Food https://t.co/seuhL2aRiV</t>
+  </si>
+  <si>
+    <t>Keşke hep böyle olsan 😒 #Allahkabuletsin #istanbul https://t.co/mkFFlo8JAn</t>
+  </si>
+  <si>
     <t>Sahurda Nerdesiniz ? ☺️ @ Varyap Meridian C blok https://t.co/vsSim0yiSL</t>
   </si>
   <si>
     <t>Godiva ( Akasya Avm ) #bugunnereyegitsem #bng @ Godiva Akasya Avm https://t.co/G4hQH2sorl</t>
   </si>
   <si>
+    <t>Koşuyoluna böyle bir mekan lazımdı hayırlı olsun ✌🏻️👏🏻 Sherbet ( Koşuyolu ) #bugunnereyegitsem https://t.co/NbzdkAt36d</t>
+  </si>
+  <si>
     <t>Sole Mare ( Çeşme ) #bugunnereyegitsem @cesmesolemare https://t.co/MPqXrraV8g</t>
   </si>
   <si>
+    <t>Herşey için teşekkürler güzeeeeeeeeeeel insan 😁😍😑 @aysehatunonal11 @ Sheraton Bursa https://t.co/wyO5fSckpf</t>
+  </si>
+  <si>
     <t>Pazar Kahvaltısı ☺️✌🏻️🎈 Cookline Pancake ( Bağdat Caddesi - Şaşkınbakkal ) #bng #bugunnereyegitsem… https://t.co/wTPuwUAXGE</t>
   </si>
   <si>
+    <t>LIVE on #Periscope: Süpermoms Şenliği - Maltepe Cevahir Otel https://t.co/yewwe1cts6</t>
+  </si>
+  <si>
     <t>Kemal Usta Waffle ( Mado ) #bugunnereyegitsem #bng #kemalustawaffle @ Kemal Usta Waffles Moda https://t.co/ywGwZS3BJW</t>
   </si>
   <si>
+    <t>Mado Emirgan #bugunnereyegitsem #bng @ Emirgan MADO http://t.co/WYDOx3FWiS</t>
+  </si>
+  <si>
+    <t>Cookline Pancake ( Bağdat Caddesi - Şaşkınbakkal ) #bng #bugunnereyegitsem #bagdatcaddesi #cookline… http://t.co/K7MwfzCq24</t>
+  </si>
+  <si>
     <t>Ankara'ya doğru yola çıktık akşam yemegine nereye gidelim, önerileri alalım ? 😁 http://t.co/2jAgemNcri</t>
   </si>
   <si>
     <t>Anı Yakala ✌️ http://t.co/6GF4QM5gpC</t>
   </si>
   <si>
+    <t>Gazebo Cafe &amp;amp; Restaurant #bugunnnereyegitsem #bng #gazebo @ Gazebo Cafe &amp;amp; Restaurant http://t.co/k1k4BpY2QO</t>
+  </si>
+  <si>
     <t>Kahvaltı önerimiz The Mono Restaurant ( Sakarya ) #bugunnereyegitsem #günaydın #sakarya #kahvaltı http://t.co/bxNraATuTP</t>
   </si>
   <si>
@@ -349,9 +642,18 @@
     <t>Akşam yemegi önerimiz Çömlek Çamlıca #bugunnereyegitsem #çömlek @ Çömlek Kurufasulye Çamlıca http://t.co/DPeXkQvfAh</t>
   </si>
   <si>
+    <t>Tatlı önerimiz Cara &amp;amp; Mocca ( Koşuyolu ) #bugunnereyegitsem @ Mocca Koşuyolu http://t.co/sOiKcomElJ</t>
+  </si>
+  <si>
+    <t>Harika sunumlarıyla ve şık dekorasyonuyla Fiyonk Bakery #bugunnereyegitsem #fiyonkbakery @ Fiyonk… http://t.co/S7zBiM3usp</t>
+  </si>
+  <si>
     <t>Kızının doğduğu gün annesi öldü iki oğlu yoğun bakımda https://t.co/dKEU2TcRey https://t.co/pNjsJ2YhaD</t>
   </si>
   <si>
+    <t>Kendisine tecavüz eden kişiyi öldüren Nevin Yıldırım için karar verildi https://t.co/M1vLVolRze https://t.co/4yNKPFrieK</t>
+  </si>
+  <si>
     <t>Çavuşoğlu'ndan Merkel'e yanıt: YPG ile aynı üslup https://t.co/Oin4k8cGKm</t>
   </si>
   <si>
@@ -361,34 +663,82 @@
     <t>Belediye Başkanının makam odasında beylik sancağı https://t.co/IHdsjtlfz6 https://t.co/arV0jQSK7H</t>
   </si>
   <si>
+    <t>RT @cnnturksndakika: #SONDAKİKA İstanbul Esenyurt'ta silahlı saldırı https://t.co/e7rUD94deC https://t.co/EmeMd0tFim</t>
+  </si>
+  <si>
+    <t>RT @CNNTURKSpor: Kyle Korver'ın kardeşi hayatını kaybetti https://t.co/u4Yt5kVp3x https://t.co/jROYktb0CA</t>
+  </si>
+  <si>
     <t>Çavuşoğlu ABD'nin açıklamasına yanıt verdi ➤ https://t.co/m6Jw2ukCQY</t>
   </si>
   <si>
     <t>Afrin'de teröristlerin tünelleri görüntüledi ➤ https://t.co/yrv9d58u0k</t>
   </si>
   <si>
+    <t>Cumhurbaşkanı Erdoğan AK Parti'li 45 milletvekiliyle görüşüyor https://t.co/ha0OnI8Ooe https://t.co/S1KBBdDjS6</t>
+  </si>
+  <si>
     <t>Türk bayrağına bastığı fotoğrafı paylaşmıştı, tutuklandı https://t.co/N4FbhZXVvc https://t.co/DDE01bfeRX</t>
   </si>
   <si>
     <t>Fransa'da üniversiteye kayyum atandı https://t.co/l0rRYNE4AI https://t.co/VmVnBGCjtQ</t>
   </si>
   <si>
+    <t>Irak'ta baharın başlangıcını simgeleyen Nevruz bayramı kutlandı, yüzlerce kişi meşalelerle Akre Tepesi'ne çıktı https://t.co/QOXcG10ofm https://t.co/ApfjaLM8sZ</t>
+  </si>
+  <si>
+    <t>Mehmed Bir Cihan Fatihi dizisinde Kosova Muharebesi nefesleri kesti! https://t.co/xqkhaiUWom</t>
+  </si>
+  <si>
+    <t>RT @CNNTURKSpor: Eczacıbaşı finale çıktı https://t.co/ZTlI77eg8w https://t.co/whBzCyvpZq</t>
+  </si>
+  <si>
     <t>Halk otobüsünde iğrenç olay! Üniversitelileri taciz edip mastürbasyon yaptı https://t.co/ZPoHf0YGf0 https://t.co/Isqp3QatvM</t>
   </si>
   <si>
     <t>Üsküdar'ın bakkal Kanber amcası 'İyilik Ödülleri' töreninde ödüle layık görülmüştü ► https://t.co/q9YsEdVdpF</t>
   </si>
   <si>
+    <t>RT @cnnturkrenk: Elon Musk'tan şaşırtan açıklama: "Babam bir şeytan" https://t.co/WRUT17YhMW https://t.co/665AwZ1Ygo</t>
+  </si>
+  <si>
+    <t>Davutoğlu, İBB Başkanlığı'na aday olacağı yolundaki iddiaya yanıt verdi https://t.co/wreN8VssOB https://t.co/5HgvZEuEWk</t>
+  </si>
+  <si>
+    <t>Muhalif Rus iş adamı Londra'da boğularak öldürüldü https://t.co/qHFtxxpECF https://t.co/gXE5rhLdep</t>
+  </si>
+  <si>
+    <t>Genelkurmay arşivinden 'Çanakkale Zaferi' fotoğrafları https://t.co/EfS97AzTv6 https://t.co/k2Dao6b0xp</t>
+  </si>
+  <si>
     <t>Bakanlık harekete geçti! Çiftlik Bank'tan sonra sırada Çılgın Tavuklar var https://t.co/7d89vkzgWE https://t.co/8ZRCGTmtoK</t>
   </si>
   <si>
+    <t>Kaza yaptı, yaralı arkadaşlarını bırakıp kaçtı https://t.co/BGVyUAn87B https://t.co/wJa8dYBZfu</t>
+  </si>
+  <si>
     <t>Afrin şehir merkezine Türk bayrağı asıldı https://t.co/phnXbR5x0G https://t.co/EdaMvoSfvK</t>
   </si>
   <si>
+    <t>Çanakkale'de bu yollar kapatılacak https://t.co/TTGligsnAK https://t.co/vlaAnLnEfz</t>
+  </si>
+  <si>
     <t>Bahçelievler'de iki araba kundaklandı https://t.co/UbarLpQJNT https://t.co/SdlNmZ76dF</t>
   </si>
   <si>
+    <t>Çanakkale'de bu yollar kapatılacak https://t.co/TTGligsnAK https://t.co/JGAnYdypP4</t>
+  </si>
+  <si>
+    <t>Polis, kaçan şüphelilerin attığı uyuşturucu maddeleri tek tek topladı https://t.co/ZkVakD0uaj https://t.co/VUxycewzS7</t>
+  </si>
+  <si>
     <t>Lise öğrencilerinden Mehmetçik'e destek  https://t.co/3KwmxZUfZL https://t.co/92ufobk5QE</t>
+  </si>
+  <si>
+    <t>CHP'li Haluk Pekşen: "Bu ittifak yasası kanuna karşı hile" https://t.co/ITIw8lCpVL https://t.co/TSYByEqQF2</t>
+  </si>
+  <si>
+    <t>RT @CNNTURKKSanat: Eski sevgili sizinle aynı gün yan salonda evlenirse… https://t.co/NGzbmgpvN8</t>
   </si>
   <si>
     <t>RT @CNNTURKSpor: Beşiktaş'ın 115. yıl forması ortalığı karıştırdı https://t.co/4b6uwEjkb9 https://t.co/ItJ6u1VLv0</t>
@@ -505,6 +855,80 @@
   </si>
   <si>
     <t>Bu yağmurlu havada 😁 #bng https://t.co/2DIqAU1BV7</t>
+  </si>
+  <si>
+    <t>01:31’de gerçekleşen 6.2 büyüklüğünde merkezüssü Muğla olan deprem, İzmir ve çevre illerden de hissedildi. https://t.co/qc2odc01yU</t>
+  </si>
+  <si>
+    <t>Avrupa Konseyi rakamları açıkladı: Türkiye, Avrupa'daki 43 ülke arasında tutuklu ve hükümlü sayısında birinci https://t.co/Rarg9BhbOP https://t.co/ILlOLlXKTS</t>
+  </si>
+  <si>
+    <t>Neden böyle bakıyorsun 🙄
+Big Chacha's - Chacha's Burger &amp;amp; Pizza &amp;amp; Steak / İstanbul #Çengelköy #burger #cuma #steak▫ https://t.co/FzlWBEIeBf</t>
+  </si>
+  <si>
+    <t>Günaydın 🎈 #SerpmeKahvaltı Hak Evrensel Hatay Sofrası #İstanbul #Florya
+☎️ 0 212 663 07 00
+💵 45₺ / Kişi Başı https://t.co/2T5bfODKtm</t>
+  </si>
+  <si>
+    <t>21 Eylül, Miladi takvim'ne göre yılın 264. (artık yıllarda 265.) günüdür. Yıl sonuna kadar kalan 101 gün vardır.</t>
+  </si>
+  <si>
+    <t>RT @CNNTURKSpor: Cedi Osman'dan mesaj var: Sevilmek kadar mutluluk verici bir şey yok https://t.co/XsPSTwuOmu https://t.co/AbU4ox0gxY</t>
+  </si>
+  <si>
+    <t>Bam's Kahvaltı - Bam's Cafe Restaurant / İstanbul ( Acıbadem ) @bams_cafe ▫️
+🕦 Çalışma Saatleri 06:00-03:00
+☎️ 0 21… https://t.co/jIRcR76VCH</t>
+  </si>
+  <si>
+    <t>Tıp Bayramı Kutlu Olsun https://t.co/Avro6F9Csi</t>
+  </si>
+  <si>
+    <t>4 Mayıs, Gregoryen Takvimi'ne göre yılın 124. (artık yıllarda 125.) günüdür. Yıl sonuna kadar kalan 241 gün vardır.</t>
+  </si>
+  <si>
+    <t>29/12/1990 - 1961 yılında işletmeden kaldırılan tramvay, İstiklal Caddesi'nde çalışmaya başladı. https://t.co/LCdbLeXCx2</t>
+  </si>
+  <si>
+    <t>Saadet Partisi lideri: "Erdoğan'a kırgınız, Gül'ün adaylığı ihtimal dahilinde" https://t.co/E0nsu50cCW https://t.co/A8lbaGAGjs</t>
+  </si>
+  <si>
+    <t>Ramazanın neşesi ☺️ Mejdul #Hurma HUЯRMACI #İstanbul #Sultanahmet
+🕦 Çalışma Saatleri 08:00 - 22:00
+💵 70₺/ Mejdul Hurma https://t.co/l7Ph4YQGEe</t>
+  </si>
+  <si>
+    <t>Chef Kahvaltı Tabağı - Burj Cafe / İstanbul ( Fenerbahçe ) 🍳
+🕦 Çalışma Saatleri 09:00-04:00
+🕦 Kahvaltı Servisi 09:0… https://t.co/OofM9hvWnD</t>
+  </si>
+  <si>
+    <t>13 Temmuz, Gregoryen Takvimi'ne göre yılın 194. (artık yıllarda 195.) günüdür. Yıl sonuna kadar kalan 171 gün vardır.</t>
+  </si>
+  <si>
+    <t>01/02/1979 - Milliyet Gazetesi Genel Yayın Yönetmeni Abdi İpekçi, suikast sonucu öldürüldü. https://t.co/L72W31Es7e</t>
+  </si>
+  <si>
+    <t>Saadet Partisi lideri: "Erdoğan'a kırgınız, Gül'ün adaylığı ihtimal dahilinde" https://t.co/E0nsu50cCW https://t.co/CslvuUBUL0</t>
+  </si>
+  <si>
+    <t>e-Devlet'te yeni bir özellik daha geliyor: Tek tıkla taşınma sonrası kurum kurum gezmeye son https://t.co/ozRvEQfUJz https://t.co/0MuKTyRDkq</t>
+  </si>
+  <si>
+    <t>Doymuyoruz 😋
+Kuzu #Kaburga &amp;amp; Metrelik #Kebap - Meşhur Kaburgacı Yaşar/ #Adana ( #Yüreğir )
+#yemekneredeyenir https://t.co/FBdKqW1V6k</t>
+  </si>
+  <si>
+    <t>15/07/1955 - Nobel Ödülü almış 18 bilim adamı, nükleer silah karşıtı Mainau Deklarasyonu'nu yayınladılar.</t>
+  </si>
+  <si>
+    <t>Hayır, diyebilir misin 🙄Yumurtalı Pastırmalı Karışık Tost - Kardeşler Büfe #İzmir #tost #MutluHaftalar https://t.co/y11yC8g58C</t>
+  </si>
+  <si>
+    <t>Yediğim en lezzetli döner gerçekten klasikleşmiş döner tadının dışına çıkmışlar 👍 Deneyimli döner… http://t.co/mDdG4pOmqb</t>
   </si>
 </sst>
 </file>
@@ -853,7 +1277,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B140"/>
+  <dimension ref="A1:B260"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1839,7 +2263,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>53</v>
+        <v>122</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -1847,7 +2271,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -1855,7 +2279,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -1863,7 +2287,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -1871,7 +2295,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -1879,7 +2303,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -1887,7 +2311,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -1895,7 +2319,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -1903,7 +2327,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -1911,7 +2335,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -1919,7 +2343,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -1927,7 +2351,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -1935,7 +2359,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -1943,7 +2367,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -1951,7 +2375,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -1959,7 +2383,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -1967,7 +2391,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -1975,7 +2399,967 @@
         <v>138</v>
       </c>
       <c r="B140" t="s">
-        <v>138</v>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="B141" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B142" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="B143" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="B144" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="B145" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="B146" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B147" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="B148" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="B149" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="B150" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="B151" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="B152" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" s="1" t="n">
+        <v>151</v>
+      </c>
+      <c r="B153" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" s="1" t="n">
+        <v>152</v>
+      </c>
+      <c r="B154" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155" s="1" t="n">
+        <v>153</v>
+      </c>
+      <c r="B155" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="B156" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="B157" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158" s="1" t="n">
+        <v>156</v>
+      </c>
+      <c r="B158" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2">
+      <c r="A159" s="1" t="n">
+        <v>157</v>
+      </c>
+      <c r="B159" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160" s="1" t="n">
+        <v>158</v>
+      </c>
+      <c r="B160" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161" s="1" t="n">
+        <v>159</v>
+      </c>
+      <c r="B161" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2">
+      <c r="A162" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="B162" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2">
+      <c r="A163" s="1" t="n">
+        <v>161</v>
+      </c>
+      <c r="B163" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2">
+      <c r="A164" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="B164" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2">
+      <c r="A165" s="1" t="n">
+        <v>163</v>
+      </c>
+      <c r="B165" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2">
+      <c r="A166" s="1" t="n">
+        <v>164</v>
+      </c>
+      <c r="B166" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2">
+      <c r="A167" s="1" t="n">
+        <v>165</v>
+      </c>
+      <c r="B167" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2">
+      <c r="A168" s="1" t="n">
+        <v>166</v>
+      </c>
+      <c r="B168" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2">
+      <c r="A169" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="B169" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2">
+      <c r="A170" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="B170" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2">
+      <c r="A171" s="1" t="n">
+        <v>169</v>
+      </c>
+      <c r="B171" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2">
+      <c r="A172" s="1" t="n">
+        <v>170</v>
+      </c>
+      <c r="B172" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2">
+      <c r="A173" s="1" t="n">
+        <v>171</v>
+      </c>
+      <c r="B173" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2">
+      <c r="A174" s="1" t="n">
+        <v>172</v>
+      </c>
+      <c r="B174" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2">
+      <c r="A175" s="1" t="n">
+        <v>173</v>
+      </c>
+      <c r="B175" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2">
+      <c r="A176" s="1" t="n">
+        <v>174</v>
+      </c>
+      <c r="B176" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2">
+      <c r="A177" s="1" t="n">
+        <v>175</v>
+      </c>
+      <c r="B177" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2">
+      <c r="A178" s="1" t="n">
+        <v>176</v>
+      </c>
+      <c r="B178" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2">
+      <c r="A179" s="1" t="n">
+        <v>177</v>
+      </c>
+      <c r="B179" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2">
+      <c r="A180" s="1" t="n">
+        <v>178</v>
+      </c>
+      <c r="B180" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2">
+      <c r="A181" s="1" t="n">
+        <v>179</v>
+      </c>
+      <c r="B181" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2">
+      <c r="A182" s="1" t="n">
+        <v>180</v>
+      </c>
+      <c r="B182" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2">
+      <c r="A183" s="1" t="n">
+        <v>181</v>
+      </c>
+      <c r="B183" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2">
+      <c r="A184" s="1" t="n">
+        <v>182</v>
+      </c>
+      <c r="B184" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2">
+      <c r="A185" s="1" t="n">
+        <v>183</v>
+      </c>
+      <c r="B185" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2">
+      <c r="A186" s="1" t="n">
+        <v>184</v>
+      </c>
+      <c r="B186" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2">
+      <c r="A187" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="B187" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2">
+      <c r="A188" s="1" t="n">
+        <v>186</v>
+      </c>
+      <c r="B188" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2">
+      <c r="A189" s="1" t="n">
+        <v>187</v>
+      </c>
+      <c r="B189" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2">
+      <c r="A190" s="1" t="n">
+        <v>188</v>
+      </c>
+      <c r="B190" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2">
+      <c r="A191" s="1" t="n">
+        <v>189</v>
+      </c>
+      <c r="B191" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2">
+      <c r="A192" s="1" t="n">
+        <v>190</v>
+      </c>
+      <c r="B192" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2">
+      <c r="A193" s="1" t="n">
+        <v>191</v>
+      </c>
+      <c r="B193" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2">
+      <c r="A194" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="B194" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2">
+      <c r="A195" s="1" t="n">
+        <v>193</v>
+      </c>
+      <c r="B195" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2">
+      <c r="A196" s="1" t="n">
+        <v>194</v>
+      </c>
+      <c r="B196" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2">
+      <c r="A197" s="1" t="n">
+        <v>195</v>
+      </c>
+      <c r="B197" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2">
+      <c r="A198" s="1" t="n">
+        <v>196</v>
+      </c>
+      <c r="B198" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2">
+      <c r="A199" s="1" t="n">
+        <v>197</v>
+      </c>
+      <c r="B199" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2">
+      <c r="A200" s="1" t="n">
+        <v>198</v>
+      </c>
+      <c r="B200" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2">
+      <c r="A201" s="1" t="n">
+        <v>199</v>
+      </c>
+      <c r="B201" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2">
+      <c r="A202" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="B202" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2">
+      <c r="A203" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="B203" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2">
+      <c r="A204" s="1" t="n">
+        <v>202</v>
+      </c>
+      <c r="B204" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2">
+      <c r="A205" s="1" t="n">
+        <v>203</v>
+      </c>
+      <c r="B205" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2">
+      <c r="A206" s="1" t="n">
+        <v>204</v>
+      </c>
+      <c r="B206" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2">
+      <c r="A207" s="1" t="n">
+        <v>205</v>
+      </c>
+      <c r="B207" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2">
+      <c r="A208" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="B208" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2">
+      <c r="A209" s="1" t="n">
+        <v>207</v>
+      </c>
+      <c r="B209" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2">
+      <c r="A210" s="1" t="n">
+        <v>208</v>
+      </c>
+      <c r="B210" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2">
+      <c r="A211" s="1" t="n">
+        <v>209</v>
+      </c>
+      <c r="B211" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2">
+      <c r="A212" s="1" t="n">
+        <v>210</v>
+      </c>
+      <c r="B212" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2">
+      <c r="A213" s="1" t="n">
+        <v>211</v>
+      </c>
+      <c r="B213" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2">
+      <c r="A214" s="1" t="n">
+        <v>212</v>
+      </c>
+      <c r="B214" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2">
+      <c r="A215" s="1" t="n">
+        <v>213</v>
+      </c>
+      <c r="B215" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2">
+      <c r="A216" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B216" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2">
+      <c r="A217" s="1" t="n">
+        <v>215</v>
+      </c>
+      <c r="B217" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2">
+      <c r="A218" s="1" t="n">
+        <v>216</v>
+      </c>
+      <c r="B218" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2">
+      <c r="A219" s="1" t="n">
+        <v>217</v>
+      </c>
+      <c r="B219" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2">
+      <c r="A220" s="1" t="n">
+        <v>218</v>
+      </c>
+      <c r="B220" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2">
+      <c r="A221" s="1" t="n">
+        <v>219</v>
+      </c>
+      <c r="B221" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2">
+      <c r="A222" s="1" t="n">
+        <v>220</v>
+      </c>
+      <c r="B222" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2">
+      <c r="A223" s="1" t="n">
+        <v>221</v>
+      </c>
+      <c r="B223" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2">
+      <c r="A224" s="1" t="n">
+        <v>222</v>
+      </c>
+      <c r="B224" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2">
+      <c r="A225" s="1" t="n">
+        <v>223</v>
+      </c>
+      <c r="B225" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2">
+      <c r="A226" s="1" t="n">
+        <v>224</v>
+      </c>
+      <c r="B226" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2">
+      <c r="A227" s="1" t="n">
+        <v>225</v>
+      </c>
+      <c r="B227" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2">
+      <c r="A228" s="1" t="n">
+        <v>226</v>
+      </c>
+      <c r="B228" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2">
+      <c r="A229" s="1" t="n">
+        <v>227</v>
+      </c>
+      <c r="B229" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2">
+      <c r="A230" s="1" t="n">
+        <v>228</v>
+      </c>
+      <c r="B230" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2">
+      <c r="A231" s="1" t="n">
+        <v>229</v>
+      </c>
+      <c r="B231" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2">
+      <c r="A232" s="1" t="n">
+        <v>230</v>
+      </c>
+      <c r="B232" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2">
+      <c r="A233" s="1" t="n">
+        <v>231</v>
+      </c>
+      <c r="B233" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2">
+      <c r="A234" s="1" t="n">
+        <v>232</v>
+      </c>
+      <c r="B234" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2">
+      <c r="A235" s="1" t="n">
+        <v>233</v>
+      </c>
+      <c r="B235" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2">
+      <c r="A236" s="1" t="n">
+        <v>234</v>
+      </c>
+      <c r="B236" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2">
+      <c r="A237" s="1" t="n">
+        <v>235</v>
+      </c>
+      <c r="B237" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2">
+      <c r="A238" s="1" t="n">
+        <v>236</v>
+      </c>
+      <c r="B238" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2">
+      <c r="A239" s="1" t="n">
+        <v>237</v>
+      </c>
+      <c r="B239" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2">
+      <c r="A240" s="1" t="n">
+        <v>238</v>
+      </c>
+      <c r="B240" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2">
+      <c r="A241" s="1" t="n">
+        <v>239</v>
+      </c>
+      <c r="B241" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2">
+      <c r="A242" s="1" t="n">
+        <v>240</v>
+      </c>
+      <c r="B242" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2">
+      <c r="A243" s="1" t="n">
+        <v>241</v>
+      </c>
+      <c r="B243" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2">
+      <c r="A244" s="1" t="n">
+        <v>242</v>
+      </c>
+      <c r="B244" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2">
+      <c r="A245" s="1" t="n">
+        <v>243</v>
+      </c>
+      <c r="B245" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2">
+      <c r="A246" s="1" t="n">
+        <v>244</v>
+      </c>
+      <c r="B246" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2">
+      <c r="A247" s="1" t="n">
+        <v>245</v>
+      </c>
+      <c r="B247" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2">
+      <c r="A248" s="1" t="n">
+        <v>246</v>
+      </c>
+      <c r="B248" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2">
+      <c r="A249" s="1" t="n">
+        <v>247</v>
+      </c>
+      <c r="B249" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2">
+      <c r="A250" s="1" t="n">
+        <v>248</v>
+      </c>
+      <c r="B250" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2">
+      <c r="A251" s="1" t="n">
+        <v>249</v>
+      </c>
+      <c r="B251" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2">
+      <c r="A252" s="1" t="n">
+        <v>250</v>
+      </c>
+      <c r="B252" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2">
+      <c r="A253" s="1" t="n">
+        <v>251</v>
+      </c>
+      <c r="B253" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2">
+      <c r="A254" s="1" t="n">
+        <v>252</v>
+      </c>
+      <c r="B254" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2">
+      <c r="A255" s="1" t="n">
+        <v>253</v>
+      </c>
+      <c r="B255" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2">
+      <c r="A256" s="1" t="n">
+        <v>254</v>
+      </c>
+      <c r="B256" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2">
+      <c r="A257" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="B257" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2">
+      <c r="A258" s="1" t="n">
+        <v>256</v>
+      </c>
+      <c r="B258" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2">
+      <c r="A259" s="1" t="n">
+        <v>257</v>
+      </c>
+      <c r="B259" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2">
+      <c r="A260" s="1" t="n">
+        <v>258</v>
+      </c>
+      <c r="B260" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>